<commit_message>
Naxxramas Bosses Status update
</commit_message>
<xml_diff>
--- a/BigWigs_Status.xlsx
+++ b/BigWigs_Status.xlsx
@@ -12,14 +12,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BigWigs!$A$1:$F$7</definedName>
-    <definedName name="Working">Variables!$A$2:$A$3</definedName>
+    <definedName name="Status">Variables!$A$2:$A$4</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="60">
   <si>
     <t>Naxxramas</t>
   </si>
@@ -36,12 +36,6 @@
     <t>Working</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>Anub'Rekhan</t>
   </si>
   <si>
@@ -70,6 +64,141 @@
   </si>
   <si>
     <t>Git Issue URL</t>
+  </si>
+  <si>
+    <t>Maexxna</t>
+  </si>
+  <si>
+    <t>Web Spray</t>
+  </si>
+  <si>
+    <t>Cocoon</t>
+  </si>
+  <si>
+    <t>Necrotic Poison</t>
+  </si>
+  <si>
+    <t>Gluth</t>
+  </si>
+  <si>
+    <t>Patchwerk</t>
+  </si>
+  <si>
+    <t>Grobbulus</t>
+  </si>
+  <si>
+    <t>Thaddius</t>
+  </si>
+  <si>
+    <t>Debuff Missing</t>
+  </si>
+  <si>
+    <t>Injected Message</t>
+  </si>
+  <si>
+    <t>Poison Cloud</t>
+  </si>
+  <si>
+    <t>Slime Spray</t>
+  </si>
+  <si>
+    <t>Fear Alert</t>
+  </si>
+  <si>
+    <t>Decimate Timer</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>needs testing</t>
+  </si>
+  <si>
+    <t>not working</t>
+  </si>
+  <si>
+    <t>Frenzy Alert</t>
+  </si>
+  <si>
+    <t>Polarity Shift</t>
+  </si>
+  <si>
+    <t>Power Surge</t>
+  </si>
+  <si>
+    <t>Throw Timer</t>
+  </si>
+  <si>
+    <t>Loatheb</t>
+  </si>
+  <si>
+    <t>Blink Cooldown</t>
+  </si>
+  <si>
+    <t>Teleport Timer</t>
+  </si>
+  <si>
+    <t>Wave Alert</t>
+  </si>
+  <si>
+    <t>Curse Timer</t>
+  </si>
+  <si>
+    <t>Decrepit Fever Alert</t>
+  </si>
+  <si>
+    <t>Spore Timer</t>
+  </si>
+  <si>
+    <t>needs DP style grp 2-8 only</t>
+  </si>
+  <si>
+    <t>Inevitable Doom Timer</t>
+  </si>
+  <si>
+    <t>needs the right timer + removecursetrigger</t>
+  </si>
+  <si>
+    <t>Instructor Razuvious</t>
+  </si>
+  <si>
+    <t>Heigan the Unclean</t>
+  </si>
+  <si>
+    <t>Noth the Plaguebringer</t>
+  </si>
+  <si>
+    <t>Unbalancing Strike</t>
+  </si>
+  <si>
+    <t>Disrupting Shout Timer</t>
+  </si>
+  <si>
+    <t>Shield Wall Timer</t>
+  </si>
+  <si>
+    <t>Gothik the Harvester</t>
+  </si>
+  <si>
+    <t>Room Arrival</t>
+  </si>
+  <si>
+    <t>Wave Timers</t>
+  </si>
+  <si>
+    <t>The Four Horsemen</t>
+  </si>
+  <si>
+    <t>Mark Timer</t>
+  </si>
+  <si>
+    <t>Meteor Timer</t>
+  </si>
+  <si>
+    <t>Holy Wrath Timer</t>
+  </si>
+  <si>
+    <t>Void Zone timer</t>
   </si>
 </sst>
 </file>
@@ -111,22 +240,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -423,19 +537,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="3" width="32.85546875" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
-    <col min="5" max="5" width="28.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="44.5703125" customWidth="1"/>
     <col min="6" max="6" width="52.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -450,13 +564,13 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -464,13 +578,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -478,13 +592,13 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -492,13 +606,13 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -506,13 +620,13 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -520,13 +634,13 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -534,13 +648,13 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -548,20 +662,544 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
         <v>10</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
         <v>15</v>
       </c>
-      <c r="D8" t="s">
-        <v>5</v>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" t="s">
+        <v>31</v>
+      </c>
+      <c r="E33" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" t="s">
+        <v>23</v>
+      </c>
+      <c r="D34" t="s">
+        <v>31</v>
+      </c>
+      <c r="E34" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" t="s">
+        <v>44</v>
+      </c>
+      <c r="D35" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36" t="s">
+        <v>49</v>
+      </c>
+      <c r="D36" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" t="s">
+        <v>50</v>
+      </c>
+      <c r="D37" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" t="s">
+        <v>51</v>
+      </c>
+      <c r="D38" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" t="s">
+        <v>52</v>
+      </c>
+      <c r="C39" t="s">
+        <v>53</v>
+      </c>
+      <c r="D39" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" t="s">
+        <v>52</v>
+      </c>
+      <c r="C40" t="s">
+        <v>54</v>
+      </c>
+      <c r="D40" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" t="s">
+        <v>55</v>
+      </c>
+      <c r="C41" t="s">
+        <v>56</v>
+      </c>
+      <c r="D41" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" t="s">
+        <v>55</v>
+      </c>
+      <c r="C42" t="s">
+        <v>51</v>
+      </c>
+      <c r="D42" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" t="s">
+        <v>57</v>
+      </c>
+      <c r="D43" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" t="s">
+        <v>55</v>
+      </c>
+      <c r="C44" t="s">
+        <v>58</v>
+      </c>
+      <c r="D44" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" t="s">
+        <v>55</v>
+      </c>
+      <c r="C45" t="s">
+        <v>59</v>
+      </c>
+      <c r="D45" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F7"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D8">
-      <formula1>Working</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D40">
+      <formula1>Status</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -571,27 +1209,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>